<commit_message>
Stats - Organic Farming - Confidence Interval
</commit_message>
<xml_diff>
--- a/project-mngmt/CA2-Planning.xlsx
+++ b/project-mngmt/CA2-Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeteixei\Documents\da-course\ca2\project-mngmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1215C26C-03CF-4975-985D-87947A12F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B270231-942C-45D1-B9D9-94A4DBE6BADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{EAF8FE12-01AA-4BD9-8723-8DB562FF7274}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{EAF8FE12-01AA-4BD9-8723-8DB562FF7274}"/>
   </bookViews>
   <sheets>
     <sheet name="CA-Tasks" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>Descriptive stats</t>
   </si>
@@ -266,12 +266,90 @@
   <si>
     <t>Content Index</t>
   </si>
+  <si>
+    <t>Data Sources</t>
+  </si>
+  <si>
+    <t>Datasets - data.gov.ie</t>
+  </si>
+  <si>
+    <t>Fertilisers</t>
+  </si>
+  <si>
+    <t>AJM05 - Fertiliser Price (Euro per Tonne) - Datasets - data.gov.ie</t>
+  </si>
+  <si>
+    <t>AJA05 - Fertiliser Price (Euro per Tonne) - Datasets - data.gov.ie</t>
+  </si>
+  <si>
+    <t>Cattle Price</t>
+  </si>
+  <si>
+    <t>AJM01 - Cattle Price (including VAT) - Datasets - data.gov.ie</t>
+  </si>
+  <si>
+    <t>Up to 2022 - Monthly basis</t>
+  </si>
+  <si>
+    <t>Up to 2021 - Yearly basis</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Performance of the agricultural sector - Statistics Explained (europa.eu)</t>
+  </si>
+  <si>
+    <t>European Countries by Population (2022) - Worldometer (worldometers.info)</t>
+  </si>
+  <si>
+    <t>Agri-environmental indicator - consumption of pesticides - Statistics Explained (europa.eu)</t>
+  </si>
+  <si>
+    <t>Overview - Agriculture - Eurostat (europa.eu)</t>
+  </si>
+  <si>
+    <t>Agri-environmental indicator - mineral fertiliser consumption - Statistics Explained (europa.eu)</t>
+  </si>
+  <si>
+    <t>Pesticides</t>
+  </si>
+  <si>
+    <t>Ireland only</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Country Factsheets (europa.eu)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,11 +371,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -353,7 +426,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +436,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,26 +509,40 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,24 +556,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -501,7 +587,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,7 +631,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,7 +711,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -715,14 +801,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
@@ -731,7 +822,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7232FDC-E07D-432E-AED6-1884B13030A9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -771,20 +862,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -793,7 +889,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22431810-BA85-4DD7-A4C9-B584993F812F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -833,20 +929,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -855,7 +956,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85898A9E-51AA-46AD-B361-5E3700265035}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -895,20 +996,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
@@ -917,7 +1023,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87674FF2-619D-4582-BDA0-022B145EF2E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -957,20 +1063,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -979,7 +1090,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93323EDA-87D3-40D9-97C3-A761CC68BCFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1019,20 +1130,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -1041,7 +1157,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F44C6487-6092-464A-B2C3-EBA23A04FC6C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1081,20 +1197,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -1103,7 +1224,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC14E8F0-93F6-4341-8D45-B07071712991}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1143,20 +1264,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
@@ -1165,7 +1291,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D74E7E-9319-4284-9BD6-94F256423941}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1205,20 +1331,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
@@ -1227,7 +1358,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81942024-F4B4-4FD1-83A3-E8F039BDAE51}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1267,20 +1398,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
@@ -1289,7 +1425,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFDE4727-E458-44CC-9B9B-D10359B4FECB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1329,20 +1465,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
@@ -1351,7 +1492,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBCFA500-111E-44D0-8FCD-C7E603446D48}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1391,20 +1532,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
@@ -1413,7 +1559,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFC76A10-E339-4AFB-A37D-0B686D8B33C1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1453,20 +1599,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
@@ -1475,7 +1626,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A7B35D-A791-43F7-A9D3-B84F6E9FEE9D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1515,20 +1666,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
@@ -1537,7 +1693,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BFBE852-88A0-49D6-823E-31B663AFCEAB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1577,20 +1733,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
@@ -1599,7 +1760,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6034897A-6471-4992-82E1-4B6EEAE3B397}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1639,20 +1800,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
@@ -1661,7 +1827,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA831A76-1200-46A5-8B20-35792F54CDFF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1701,20 +1867,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1056" name="Check Box 32" hidden="1">
@@ -1723,7 +1894,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0235BBB8-E482-429D-ACEB-80CDA581D5CD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1763,20 +1934,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1057" name="Check Box 33" hidden="1">
@@ -1785,7 +1961,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8142BCE2-6196-433E-B470-4B80A4D11C92}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1825,20 +2001,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
@@ -1847,7 +2028,7 @@
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6787004-E915-4F25-8637-260ACBB1435D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1887,20 +2068,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1059" name="Check Box 35" hidden="1">
@@ -1909,7 +2095,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5B6B9F0-AFE6-4CAA-894A-644FFACF2F67}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1949,20 +2135,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1060" name="Check Box 36" hidden="1">
@@ -1971,7 +2162,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967CBAF3-0475-4D1A-ABE1-2C011D76E691}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2011,7 +2202,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2027,7 +2218,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>195263</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>23812</xdr:rowOff>
+          <xdr:rowOff>23813</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -2094,11 +2285,11 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>538162</xdr:colOff>
+          <xdr:colOff>538163</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>280988</xdr:rowOff>
         </xdr:to>
@@ -2110,7 +2301,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E786E94-15B0-2C65-00D3-8D1B906ED5B5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2156,14 +2347,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
@@ -2172,7 +2368,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8077EDAC-715A-4771-A8ED-FC80C98854CD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2212,20 +2408,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>14288</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
@@ -2234,7 +2435,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1EF0A2B-1CB8-400A-8366-82292A004A68}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2274,20 +2475,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>280988</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
@@ -2296,7 +2502,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9200BFA6-27D6-464C-9CC4-122B2CDC1CF8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2336,20 +2542,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>280988</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2055" name="Check Box 7" hidden="1">
@@ -2358,7 +2569,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D7AFE7-DB07-4033-8B4B-2F854DC22BDA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2398,20 +2609,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>280988</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2056" name="Check Box 8" hidden="1">
@@ -2420,7 +2636,7 @@
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{660738AA-5234-40C5-B5C6-8B874DB918B2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2460,20 +2676,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>14288</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2057" name="Check Box 9" hidden="1">
@@ -2482,7 +2703,7 @@
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F3EFE9F-6D70-4E9B-8924-077A033BFCE0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2522,20 +2743,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>280988</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
@@ -2544,7 +2770,7 @@
                   <a14:compatExt spid="_x0000_s2058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D689EE15-602F-4D00-9AE9-B67A1922E3D0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2584,20 +2810,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>280988</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2059" name="Check Box 11" hidden="1">
@@ -2606,7 +2837,7 @@
                   <a14:compatExt spid="_x0000_s2059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6184843E-1E22-4BB6-A753-8B4CCE780DC5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2646,20 +2877,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
@@ -2668,7 +2904,7 @@
                   <a14:compatExt spid="_x0000_s2060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1602E8EE-376F-4021-8E7B-30043E7711A8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2708,20 +2944,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2061" name="Check Box 13" hidden="1">
@@ -2730,7 +2971,7 @@
                   <a14:compatExt spid="_x0000_s2061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20FE83FC-B2A2-43D2-A2F1-9F184910DAAE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2770,20 +3011,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>4763</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2062" name="Check Box 14" hidden="1">
@@ -2792,7 +3038,7 @@
                   <a14:compatExt spid="_x0000_s2062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E9F3859-644B-4FD9-9A07-88A373C6227D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2832,20 +3078,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>66676</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="347662" cy="214312"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>538163</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>4763</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2063" name="Check Box 15" hidden="1">
@@ -2854,7 +3105,7 @@
                   <a14:compatExt spid="_x0000_s2063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5AF3A2B-E51E-4361-ABBD-EF7132D732B2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2894,7 +3145,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2902,7 +3153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3201,8 +3452,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3212,231 +3463,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="9"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="9"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A12" s="9"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="9"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A15" s="9"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="114" x14ac:dyDescent="0.45">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="114" x14ac:dyDescent="0.45">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="1"/>
@@ -3952,7 +4203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD290F53-7692-49DD-BF58-BDC6BCC01CAD}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3962,67 +4213,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="1"/>
@@ -4353,24 +4604,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6A9E6-253A-4C9D-826D-AADB48782758}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="22"/>
+      <c r="B8" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="23"/>
+      <c r="B9" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:A9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="https://data.gov.ie/dataset?theme=Agriculture&amp;page=9" xr:uid="{3D1C5824-376C-4307-8004-3CF2B72158F2}"/>
+    <hyperlink ref="B7" r:id="rId2" display="https://data.gov.ie/dataset/ajm05-fertiliser-price-euro-per-tonne?package_type=dataset" xr:uid="{C3EB095D-A644-47E3-A659-3479263B46FC}"/>
+    <hyperlink ref="B8" r:id="rId3" display="https://data.gov.ie/dataset/aja05-fertiliser-price-euro-per-tonne?package_type=dataset" xr:uid="{406062A0-4882-4F38-AC8E-A376D173448A}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://data.gov.ie/dataset/ajm01-cattle-price-including-vat?package_type=dataset" xr:uid="{60E00138-CEEC-41BF-918A-640475AD2BBF}"/>
+    <hyperlink ref="B5" r:id="rId5" display="https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Agri-environmental_indicator_-_consumption_of_pesticides" xr:uid="{22A9BB96-A775-4C23-A291-402334E426F3}"/>
+    <hyperlink ref="B2" r:id="rId6" display="https://ec.europa.eu/eurostat/web/agriculture/overview" xr:uid="{AE27D87F-7D40-4261-A0A2-BBD00715B922}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Agri-environmental_indicator_-_mineral_fertiliser_consumption" xr:uid="{80F2A6F0-938D-4605-9110-4D08F3A738D7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA20F89-DF0F-41E9-A21E-B3F94542F694}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Performance_of_the_agricultural_sector" xr:uid="{817D2454-263B-4012-B73C-3091CD8D60E2}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://www.worldometers.info/population/countries-in-europe-by-population/" xr:uid="{2ECA6538-67B0-4553-9DDB-75FF16842A21}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://agridata.ec.europa.eu/extensions/CountryFactsheets/CountryFactsheets.html?memberstate=Ireland" xr:uid="{A50D8379-8FE1-4841-9C54-49E3F7E3753C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Stats - Import/Export analysis - Start of food price inflation
</commit_message>
<xml_diff>
--- a/project-mngmt/CA2-Planning.xlsx
+++ b/project-mngmt/CA2-Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeteixei\Documents\da-course\ca2\project-mngmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B270231-942C-45D1-B9D9-94A4DBE6BADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F855E5-0EAF-483A-9829-F5CC599A7853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{EAF8FE12-01AA-4BD9-8723-8DB562FF7274}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>Descriptive stats</t>
   </si>
@@ -343,6 +344,9 @@
   </si>
   <si>
     <t>Country Factsheets (europa.eu)</t>
+  </si>
+  <si>
+    <t>Kruskal, Shapiro, Mannwhitneyu, Shapiro</t>
   </si>
 </sst>
 </file>
@@ -538,6 +542,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -556,9 +563,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3450,19 +3454,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A06A931-17E5-4DDD-AAD1-957C789B8BF3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="48.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.86328125" customWidth="1"/>
+    <col min="5" max="5" width="33.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>54</v>
       </c>
@@ -3476,8 +3481,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3488,8 +3493,8 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="15"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3498,8 +3503,8 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3508,8 +3513,8 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="15"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3517,9 +3522,12 @@
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3528,8 +3536,8 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -3538,8 +3546,8 @@
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -3548,34 +3556,34 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="15"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A12" s="15"/>
+    <row r="12" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -3584,26 +3592,26 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="15"/>
+    <row r="13" spans="1:5" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="13"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A15" s="15"/>
+    <row r="15" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
@@ -3612,8 +3620,8 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="16"/>
+    <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="19"/>
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
@@ -3621,7 +3629,7 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3633,25 +3641,25 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="12"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="12"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="114" x14ac:dyDescent="0.45">
-      <c r="A20" s="12"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
@@ -3661,7 +3669,7 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="114" x14ac:dyDescent="0.45">
-      <c r="A21" s="12"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
@@ -3671,7 +3679,7 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3683,7 +3691,7 @@
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A23" s="12"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
@@ -4623,7 +4631,7 @@
       <c r="A1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C1" t="s">
@@ -4631,7 +4639,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C2" t="s">
@@ -4639,22 +4647,22 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B3" s="18"/>
+      <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -4662,7 +4670,7 @@
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -4675,7 +4683,7 @@
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -4692,7 +4700,7 @@
       <c r="A7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4707,7 +4715,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="22"/>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -4722,7 +4730,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="23"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -4760,17 +4768,17 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ML - Sentiment analysis
</commit_message>
<xml_diff>
--- a/project-mngmt/CA2-Planning.xlsx
+++ b/project-mngmt/CA2-Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeteixei\Documents\da-course\ca2\project-mngmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DA626-4043-4E90-B024-AA5ABAB59E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944ED81C-7CBB-4337-98E7-569CBA58EAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{EAF8FE12-01AA-4BD9-8723-8DB562FF7274}"/>
   </bookViews>
@@ -3606,8 +3606,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
ML Comments and Dataset Logic - Fixes in the Stats notebook
</commit_message>
<xml_diff>
--- a/project-mngmt/CA2-Planning.xlsx
+++ b/project-mngmt/CA2-Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeteixei\Documents\da-course\ca2\project-mngmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944ED81C-7CBB-4337-98E7-569CBA58EAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88331133-9170-4EBA-9371-4369E79D5BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{EAF8FE12-01AA-4BD9-8723-8DB562FF7274}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>Descriptive stats</t>
   </si>
@@ -353,6 +352,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Naïve Bayes, Logistic Regression</t>
   </si>
 </sst>
 </file>
@@ -558,6 +560,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,11 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -617,7 +619,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,7 +751,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,7 +775,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>566737</xdr:colOff>
+          <xdr:colOff>566738</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>261938</xdr:rowOff>
         </xdr:to>
@@ -903,13 +905,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>47624</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>614362</xdr:colOff>
+          <xdr:colOff>614363</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>304799</xdr:rowOff>
+          <xdr:rowOff>304800</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1236,13 +1238,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>52387</xdr:colOff>
+          <xdr:colOff>52388</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>314324</xdr:rowOff>
+          <xdr:rowOff>314325</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>347662</xdr:colOff>
+          <xdr:colOff>347663</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
@@ -1303,13 +1305,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>52387</xdr:colOff>
+          <xdr:colOff>52388</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>309562</xdr:colOff>
+          <xdr:colOff>309563</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -1443,7 +1445,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>500062</xdr:colOff>
+          <xdr:colOff>500063</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>242888</xdr:rowOff>
         </xdr:to>
@@ -1847,7 +1849,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>347663</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>176212</xdr:rowOff>
+          <xdr:rowOff>176213</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1908,13 +1910,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>57150</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>171449</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>314325</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>23811</xdr:rowOff>
+          <xdr:rowOff>23813</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2238,14 +2240,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="742950" cy="228600"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>276225</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1061" name="Check Box 37" hidden="1">
@@ -2254,7 +2261,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A2AA2E9-32AE-476D-8374-B34740DA2B27}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2294,20 +2301,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>47625</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="519112" cy="214313"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>566738</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>261938</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1062" name="Check Box 38" hidden="1">
@@ -2316,7 +2328,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC8D46FE-87A0-4BE8-8D47-D56B60441E2E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2356,7 +2368,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3606,8 +3618,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3632,7 +3644,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3641,43 +3653,43 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="24" t="b">
+      <c r="D2" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="15"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="24" t="b">
+      <c r="D3" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24" t="b">
+      <c r="D4" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="24" t="b">
+      <c r="D5" s="15" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -3685,14 +3697,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="24" t="b">
+      <c r="D6" s="15" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="s">
@@ -3700,38 +3712,41 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="24" t="b">
+      <c r="D7" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="18"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="24" t="b">
-        <v>0</v>
+      <c r="D8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="18"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="24" t="b">
+      <c r="D9" s="15" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="s">
@@ -3739,78 +3754,78 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="18"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="24" t="b">
+      <c r="C10" s="19"/>
+      <c r="D10" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="18"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="24" t="b">
+      <c r="C11" s="19"/>
+      <c r="D11" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A12" s="18"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="24" t="b">
-        <v>0</v>
+      <c r="D12" s="15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="18"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="24" t="b">
+      <c r="D13" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="24" t="b">
+      <c r="C14" s="19"/>
+      <c r="D14" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A15" s="18"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="24" t="b">
+      <c r="D15" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="19"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="24" t="b">
+      <c r="D16" s="15" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
@@ -3818,7 +3833,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3827,7 +3842,7 @@
       <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="24" t="b">
+      <c r="D17" s="15" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
@@ -3835,53 +3850,53 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="15"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="24" t="b">
+      <c r="D18" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="15"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="24" t="b">
+      <c r="C19" s="23"/>
+      <c r="D19" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="114" x14ac:dyDescent="0.45">
-      <c r="A20" s="15"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="24" t="b">
+      <c r="D20" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="114" x14ac:dyDescent="0.45">
-      <c r="A21" s="15"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="24" t="b">
+      <c r="D21" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3890,29 +3905,29 @@
       <c r="C22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="24" t="b">
+      <c r="D22" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A23" s="15"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="24" t="b">
+      <c r="D23" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="17">
         <f>COUNTIF(D2:D23,TRUE)/COUNTIF(D2:D23,"&lt;&gt;")</f>
-        <v>0.40909090909090912</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -4956,7 +4971,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -4973,7 +4988,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="22"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="13" t="s">
         <v>61</v>
       </c>
@@ -4988,7 +5003,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="23"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="13" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Final commit - Deadline
</commit_message>
<xml_diff>
--- a/project-mngmt/CA2-Planning.xlsx
+++ b/project-mngmt/CA2-Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeteixei\Documents\da-course\ca2\project-mngmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFDE6D1-E7AF-4463-8853-9A248291632E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB1AB8-B95B-4190-A2FF-5117298F309F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{EAF8FE12-01AA-4BD9-8723-8DB562FF7274}"/>
   </bookViews>
@@ -632,11 +632,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -680,7 +680,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -744,7 +744,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -772,7 +772,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3884,7 +3884,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3970,7 +3970,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>82</v>
@@ -4012,7 +4012,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>82</v>
@@ -4081,7 +4081,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>82</v>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>82</v>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D24" s="17">
         <f>COUNTIF(D2:D23,TRUE)/COUNTIF(D2:D23,"&lt;&gt;")</f>
-        <v>0.81818181818181823</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>